<commit_message>
Update Liste de composant KANE KANIA MARTIN.xlsx
</commit_message>
<xml_diff>
--- a/Dossiers/Liste de composant KANE KANIA MARTIN.xlsx
+++ b/Dossiers/Liste de composant KANE KANIA MARTIN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IUT\SAE-S5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\GitHub\SAE-S5\Dossiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB352BCA-C84D-410F-8270-6BA3E2915596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD54C1C-538B-4F2A-86B4-79BB4ACC9B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{D77634F6-E77F-462F-9E70-584C282198EA}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{D77634F6-E77F-462F-9E70-584C282198EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Nom du composant</t>
   </si>
@@ -69,6 +69,27 @@
   </si>
   <si>
     <t>haut parleur 3w  8ohms</t>
+  </si>
+  <si>
+    <t>entretoises</t>
+  </si>
+  <si>
+    <t>connecteur femelle jack DC 5,5X2,1</t>
+  </si>
+  <si>
+    <t>chargeur 12v</t>
+  </si>
+  <si>
+    <t>ressorts (X5)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/BIlinli-DC-005-Connecteur-5-5x2-1mm-Barrel/dp/B082B7VQRY/ref=sr_1_6?__mk_fr_FR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dib=eyJ2IjoiMSJ9.zaqWM5kZHUhQQR3Ar-_dPFqrPcrjUAWIURpgQoX8U4pKqx9iJOyQmh8juWfIply3MGozRWA4PK5UpUi6uHCja_YsyH3aIb02I321vk5zIY0zZrQo0s-_rcP59bzlGbUn3jXrk-PYGWoNa-F-5LTEYbHK9u-Qu3S-paWdsLBG8eU1d6oI1D5kuIkblKNC9bjMXY-NbJPzpQ5Z6PnpOCU6Y2fHgQs9qCvxiMC2G95dktSBfqcqL0Oeq9AvS1Cm-QWJb5yTROig-u1Veq1XgvrIeydLv7gQLXi-ckNoXkAq_5k2Goki83N-cCKUCYsvGkQXMdChRscXAuSHN7zVTiB4I1VhOMp0eVQ3LzpFCiTdLgKQPikedw7iBBE7KbatGXVx2D_yQLIKvAJyr8gAgesbjE6H1z0uCGF7OwR8jupltClHrsQ4o_qMF9-yYjMGd9fD.GwQgSGeDNs8PSCiMyg35wu3cF7VkPHT0IVfdAYKmNRU&amp;dib_tag=se&amp;keywords=dc+jack+pcb&amp;qid=1740840369&amp;sr=8-6</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/Adaptateur-Alimentation-dalimentation-adaptateurs-convertisseur/dp/B09KNC7SDQ/ref=sr_1_5?dib=eyJ2IjoiMSJ9.kh4ME1fgLwcNRdIka5gVXrYsbm_HulQVUeVuKNMClm8kezgqD7oLYXZEnvZhdBtjKVmlWR_ygZ47e2nU3gspl7XBdliMYf5fC_xpPFQp4p4zdewgWqvd9Ztq_yhXsBIQPHK9tyvEENLNJBp6HMmjhLIoaLHOeYguf6Pe40BN_MimRcglxRfbslwaohYN5KlC7XeBYpvazD_MMvZSYMF1LUUodypRUWlFoDmgu4qjOvG3QU4wBi_TmTjXj5H_GzkbjUMp1ByKSg3463KvWQs4A-8MfTfp8Jt-j8qL7jwZO9wv2mbRI3syJ0x0MFgpKITtZXvGRxiolqiw0f7XFFc9P2wwoA0Xi03zowoz5NAV5y8r04eN34F3d36OsWB0umprTbaXlaY1RsjP_8t2GAV269poIuAMs7Qx47t51wI3Hhrq5XRGMpno8_4ibh5r6gwe.OO38cFMDgwd4r9Wqpo2xCEjt3winmd1ijKS_Ee3Ozqc&amp;dib_tag=se&amp;keywords=transformateur%2B12v&amp;qid=1740840232&amp;sr=8-5&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://fr.rs-online.com/web/p/ressorts-de-compression/0751512?searchId=1b93648f-6bca-46c3-8c8a-d5bf4eda4f0b&amp;gb=s</t>
   </si>
 </sst>
 </file>
@@ -122,7 +143,7 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -139,7 +160,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -455,20 +476,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF56196-CBD8-4EF2-99B7-FFFC59C11BB7}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -490,7 +511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -501,7 +522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -512,7 +533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -521,6 +542,44 @@
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>3.49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>11.97</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>6.86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>